<commit_message>
Question 6, dropdown B87 done, beginning to fill in budget table
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adaly\Documents\DA11\Excel\lookups-exercise-AdellAD4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D83275-CABA-4EB2-88A0-9549D001A9F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7007EA-0B1B-447E-9681-43DAF4171AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -237,15 +237,6 @@
     <t>Trustee</t>
   </si>
   <si>
-    <t>Question 3</t>
-  </si>
-  <si>
-    <t>Question 4</t>
-  </si>
-  <si>
-    <t>Question 5</t>
-  </si>
-  <si>
     <t>Question 6</t>
   </si>
   <si>
@@ -304,6 +295,15 @@
   </si>
   <si>
     <t>Actual spending amount - budget amount for fiscal year 2019</t>
+  </si>
+  <si>
+    <t>Question 5 (Index + Match)</t>
+  </si>
+  <si>
+    <t>Question 4 (XLOOKUP)</t>
+  </si>
+  <si>
+    <t>Question 3 (VLOOKUP)</t>
   </si>
 </sst>
 </file>
@@ -1178,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4257,7 +4257,7 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -4283,8 +4283,12 @@
         <v>-36209.630000000005</v>
       </c>
       <c r="C56">
-        <f>_xlfn.XLOOKUP("Community Education Commission", A2:A52, I2:I52)</f>
+        <f>VLOOKUP(A10,A2:I52,9)</f>
         <v>-27292.159999999974</v>
+      </c>
+      <c r="D56">
+        <f>VLOOKUP(A10,A2:N52,14)</f>
+        <v>-9181.0800000000163</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
@@ -4296,8 +4300,12 @@
         <v>0</v>
       </c>
       <c r="C57">
-        <f>_xlfn.XLOOKUP("Community Oversight Board", A2:A52, I2:I52)</f>
-        <v>0</v>
+        <f>VLOOKUP(A11,A2:I52,9)</f>
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <f>VLOOKUP(A11,A2:N52,14)</f>
+        <v>-311228.08999999997</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
@@ -4309,8 +4317,12 @@
         <v>-149396.10000000987</v>
       </c>
       <c r="C58">
-        <f>_xlfn.XLOOKUP("Election Commission", A2:A52, I2:I52)</f>
+        <f>VLOOKUP(A18,A2:I52,9)</f>
         <v>-189254.06000000006</v>
+      </c>
+      <c r="D58">
+        <f>VLOOKUP(A18,A2:N52,14)</f>
+        <v>-374962.91000000015</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
@@ -4322,8 +4334,12 @@
         <v>-12230.810000000056</v>
       </c>
       <c r="C59">
-        <f>_xlfn.XLOOKUP("Historical Commission", A2:A52, I2:I52)</f>
+        <f>VLOOKUP(A24,A2:I52,9)</f>
         <v>-45485.580000000075</v>
+      </c>
+      <c r="D59">
+        <f>VLOOKUP(A24,A2:N52,14)</f>
+        <v>-72.879999999888241</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
@@ -4335,8 +4351,12 @@
         <v>-4950.4699999999721</v>
       </c>
       <c r="C60">
-        <f>_xlfn.XLOOKUP("Human Relations Commission", A2:A52, I2:I52)</f>
+        <f>VLOOKUP(A25,A2:I52,9)</f>
         <v>-8005.7900000010268</v>
+      </c>
+      <c r="D60">
+        <f>VLOOKUP(A25,A2:N52,14)</f>
+        <v>-1724.9000000000233</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
@@ -4348,13 +4368,17 @@
         <v>-184239.79000001028</v>
       </c>
       <c r="C61">
-        <f>_xlfn.XLOOKUP("Planning Commission", A2:A52, I2:I52)</f>
+        <f>VLOOKUP(A41,A2:I52,9)</f>
         <v>-133456.33000001032</v>
+      </c>
+      <c r="D61">
+        <f>VLOOKUP(A41,A2:N52,14)</f>
+        <v>-82077.349999999627</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
@@ -4375,35 +4399,107 @@
       <c r="A65" t="s">
         <v>24</v>
       </c>
+      <c r="B65">
+        <f>_xlfn.XLOOKUP("Community Education Commission", A2:A52, D2:D52)</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="C65">
+        <f>_xlfn.XLOOKUP("Community Education Commission", A2:A52, I2:I52)</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="D65">
+        <f>_xlfn.XLOOKUP("Community Education Commission", A2:A52, N2:N52)</f>
+        <v>-9181.0800000000163</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>25</v>
       </c>
+      <c r="B66">
+        <f>_xlfn.XLOOKUP("Community Oversight Board", A2:A52, D2:D52)</f>
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <f>_xlfn.XLOOKUP("Community Oversight Board", A2:A52, I2:I52)</f>
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <f>_xlfn.XLOOKUP("Community Oversight Board", A2:A52, N2:N52)</f>
+        <v>-311228.08999999997</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>32</v>
       </c>
+      <c r="B67">
+        <f>_xlfn.XLOOKUP("Election Commission", A2:A52, D2:D52)</f>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C67">
+        <f>_xlfn.XLOOKUP("Election Commission", A2:A52, I2:I52)</f>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="D67">
+        <f>_xlfn.XLOOKUP("Election Commission", A2:A52, N2:N52)</f>
+        <v>-374962.91000000015</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>38</v>
       </c>
+      <c r="B68">
+        <f>_xlfn.XLOOKUP("Historical Commission", A2:A52, D2:D52)</f>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C68">
+        <f>_xlfn.XLOOKUP("Historical Commission", A2:A52, I2:I52)</f>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="D68">
+        <f>_xlfn.XLOOKUP("Historical Commission", A2:A52, N2:N52)</f>
+        <v>-72.879999999888241</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>39</v>
       </c>
+      <c r="B69">
+        <f>_xlfn.XLOOKUP("Human Relations Commission", A2:A52, D2:D52)</f>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C69">
+        <f>_xlfn.XLOOKUP("Human Relations Commission", A2:A52, I2:I52)</f>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="D69">
+        <f>_xlfn.XLOOKUP("Human Relations Commission", A2:A52, N2:N52)</f>
+        <v>-1724.9000000000233</v>
+      </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>55</v>
       </c>
+      <c r="B70">
+        <f>_xlfn.XLOOKUP("Planning Commission", A2:A52, D2:D52)</f>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C70">
+        <f>_xlfn.XLOOKUP("Planning Commission", A2:A52, I2:I52)</f>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="D70">
+        <f>_xlfn.XLOOKUP("Planning Commission", A2:A52, N2:N52)</f>
+        <v>-82077.349999999627</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -4424,35 +4520,107 @@
       <c r="A74" t="s">
         <v>24</v>
       </c>
+      <c r="B74">
+        <f>INDEX(D2:D52,MATCH("Community Education Commission",A2:A52,0))</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="C74">
+        <f>INDEX(I2:I52,MATCH("Community Education Commission",A2:A52,0))</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="D74">
+        <f>INDEX(N2:N52,MATCH("Community Education Commission",A2:A52,0))</f>
+        <v>-9181.0800000000163</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>25</v>
       </c>
+      <c r="B75">
+        <f>INDEX(D2:D52,MATCH("Community Oversight Board",A2:A52,0))</f>
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <f>INDEX(I2:I52,MATCH("Community Oversight Board",A2:A52,0))</f>
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <f>INDEX(N2:N52,MATCH("Community Oversight Board",A2:A52,0))</f>
+        <v>-311228.08999999997</v>
+      </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>32</v>
       </c>
+      <c r="B76">
+        <f>INDEX(D2:D52,MATCH("Election Commission",A2:A52,0))</f>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C76">
+        <f>INDEX(I2:I52,MATCH("Election Commission",A2:A52,0))</f>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="D76">
+        <f>INDEX(N2:N52,MATCH("Election Commission",A2:A52,0))</f>
+        <v>-374962.91000000015</v>
+      </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>38</v>
       </c>
+      <c r="B77">
+        <f>INDEX(D2:D52,MATCH("Historical Commission",A2:A52,0))</f>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C77">
+        <f>INDEX(I2:I52,MATCH("Historical Commission",A2:A52,0))</f>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="D77">
+        <f>INDEX(N2:N52,MATCH("Historical Commission",A2:A52,0))</f>
+        <v>-72.879999999888241</v>
+      </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>39</v>
       </c>
+      <c r="B78">
+        <f>INDEX(D2:D52,MATCH("Human Relations Commission",A2:A52,0))</f>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C78">
+        <f>INDEX(I2:I52,MATCH("Human Relations Commission",A2:A52,0))</f>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="D78">
+        <f>INDEX(N2:N52,MATCH("Human Relations Commission",A2:A52,0))</f>
+        <v>-1724.9000000000233</v>
+      </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>55</v>
       </c>
+      <c r="B79">
+        <f>INDEX(D2:D52,MATCH("Planning Commission",A2:A52,0))</f>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C79">
+        <f>INDEX(I2:I52,MATCH("Planning Commission",A2:A52,0))</f>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="D79">
+        <f>INDEX(N2:N52,MATCH("Planning Commission",A2:A52,0))</f>
+        <v>-82077.349999999627</v>
+      </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -4462,41 +4630,44 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>73</v>
-      </c>
-      <c r="B84" s="6"/>
+        <v>70</v>
+      </c>
+      <c r="B84" s="6">
+        <f>INDEX(B2:B52,MATCH("Administrative",A2:A52,0))</f>
+        <v>356640100</v>
+      </c>
       <c r="C84" s="6"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B89" s="7">
         <v>1</v>
@@ -4515,24 +4686,24 @@
         <v>0</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D90" s="8" t="s">
         <v>0</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F90" s="8" t="s">
         <v>0</v>
       </c>
       <c r="G90" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C91" s="5"/>
       <c r="E91" s="5"/>
@@ -4540,7 +4711,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C92" s="5"/>
       <c r="E92" s="5"/>
@@ -4548,7 +4719,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C93" s="5"/>
       <c r="E93" s="5"/>
@@ -4556,12 +4727,12 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B96" s="7">
         <v>1</v>
@@ -4580,24 +4751,24 @@
         <v>0</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D97" s="8" t="s">
         <v>0</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F97" s="8" t="s">
         <v>0</v>
       </c>
       <c r="G97" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C98" s="4"/>
       <c r="E98" s="4"/>
@@ -4606,7 +4777,7 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C99" s="4"/>
       <c r="E99" s="4"/>
@@ -4615,7 +4786,7 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C100" s="4"/>
       <c r="E100" s="4"/>
@@ -4624,7 +4795,7 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83 B87" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
       <formula1>$A$2:$A$52</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
@@ -4652,7 +4823,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -4660,7 +4831,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -4668,7 +4839,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -4676,7 +4847,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -4684,7 +4855,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -4692,7 +4863,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -4700,7 +4871,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -4708,7 +4879,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -4716,7 +4887,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -4724,7 +4895,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Not understanding how to do questions 7-9
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adaly\Documents\DA11\Excel\lookups-exercise-AdellAD4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07348605-B59F-4EEA-BC70-4257B59DD6A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7FC794-2E79-4EDB-9028-9862A1A5D0B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="91">
   <si>
     <t>Department</t>
   </si>
@@ -304,6 +304,9 @@
   </si>
   <si>
     <t>Question 3 (VLOOKUP)</t>
+  </si>
+  <si>
+    <t>XLOOKUP(,E2:E52,</t>
   </si>
 </sst>
 </file>
@@ -2496,8 +2499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B81" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5597,7 +5600,7 @@
         <v>24</v>
       </c>
       <c r="B56">
-        <f>VLOOKUP(A10,A2:D52,4)</f>
+        <f>VLOOKUP($A10,$A$2:$P$52,MATCH(D1,$A$1:$P$1,0))</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="C56">
@@ -6042,6 +6045,9 @@
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>70</v>
+      </c>
+      <c r="B91" t="s">
+        <v>90</v>
       </c>
       <c r="C91" s="5"/>
       <c r="E91" s="5"/>

</xml_diff>